<commit_message>
Commit com as requisições:
- Saída de Results_Excel.py foi arrumada de acordo com a solicitação do Giovani;

- Ínicio da simulação pode ser qualquer dia e a simulação pode durar até 365 dias
</commit_message>
<xml_diff>
--- a/Excel_Results/Cronograma_Sintetizado.xlsx
+++ b/Excel_Results/Cronograma_Sintetizado.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G157"/>
+  <dimension ref="A1:G161"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,20 +478,20 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>14/06/2019</t>
+          <t>01/09/2021</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>12/07/2019</t>
+          <t>23/10/2021</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>MANUTENÇÃO CORRETIVA VEDAÇÃO DO EIXO</t>
+          <t>(1) CAVITAÇÃO (2) SUBSTITUIÇÃO VEDAÇÃO MUNHÕES PALHETAS (3) PARADA DA ILHA - TRANSFORMADOR (4) MANUTENÇÃO NO CDG</t>
         </is>
       </c>
       <c r="F2" t="inlineStr"/>
@@ -505,20 +505,20 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>30/07/2019</t>
+          <t>05/11/2021</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>20/09/2019</t>
+          <t>17/11/2021</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>53</v>
+        <v>13</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>(1) CAVITAÇÃO (2) SUBSTITUIÇÃO VEDAÇÃO MUNHÕES PALHETAS (3) PARADA DA ILHA - TRANSFORMADOR (4) MANUTENÇÃO NO CDG</t>
+          <t>MANUTENÇÃO CORRETIVA RETIRADA DE VAZAMENTO DISTRIBUIDOR E VÁLVULAS DE DRENAGEM</t>
         </is>
       </c>
       <c r="F3" t="inlineStr"/>
@@ -532,47 +532,43 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>28/09/2019</t>
+          <t>12/06/2022</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>16/10/2019</t>
+          <t>28/07/2022</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>19</v>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>BIELISMO ROTOR KAPLAN</t>
-        </is>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>ROUHSN_13P8_UG01</t>
+          <t>ROUHSN_13P8_UG02</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>18/11/2019</t>
+          <t>25/08/2021</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>30/11/2019</t>
+          <t>10/09/2021</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>MANUTENÇÃO CORRETIVA RETIRADA DE VAZAMENTO DISTRIBUIDOR E VÁLVULAS DE DRENAGEM</t>
+          <t>VEDAÇÃO DO EIXO</t>
         </is>
       </c>
       <c r="F5" t="inlineStr"/>
@@ -586,20 +582,20 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>11/06/2019</t>
+          <t>26/09/2021</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>27/06/2019</t>
+          <t>05/12/2021</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>17</v>
+        <v>71</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>VEDAÇÃO DO EIXO</t>
+          <t>(1) CAVITAÇÃO (2) REFORÇO ARO CAMARA (3) ALTERAÇÃO DA PLATAFORMA DO ARO CÂMARA</t>
         </is>
       </c>
       <c r="F6" t="inlineStr"/>
@@ -613,20 +609,20 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>07/07/2019</t>
+          <t>12/12/2021</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>24/07/2019</t>
+          <t>27/12/2021</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>(1) BIELISMO ROTOR KAPLAN (2) MANUTENÇÃO NO CDG (3) PARADA DA ILHA - TRANSFORMADOR</t>
+          <t>JUNTA DESLIZANTE</t>
         </is>
       </c>
       <c r="F7" t="inlineStr"/>
@@ -640,20 +636,20 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>30/07/2019</t>
+          <t>27/06/2022</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>08/10/2019</t>
+          <t>14/07/2022</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>71</v>
+        <v>18</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>(1) CAVITAÇÃO (2) REFORÇO ARO CAMARA (3) ALTERAÇÃO DA PLATAFORMA DO ARO CÂMARA</t>
+          <t>(1) BIELISMO ROTOR KAPLAN (2) MANUTENÇÃO NO CDG (3) PARADA DA ILHA - TRANSFORMADOR</t>
         </is>
       </c>
       <c r="F8" t="inlineStr"/>
@@ -662,25 +658,25 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>ROUHSN_13P8_UG02</t>
+          <t>ROUHSN_13P8_UG03</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>27/11/2019</t>
+          <t>11/09/2021</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>12/12/2019</t>
+          <t>15/11/2021</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>16</v>
+        <v>66</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>JUNTA DESLIZANTE</t>
+          <t>CAVITAÇÃO</t>
         </is>
       </c>
       <c r="F9" t="inlineStr"/>
@@ -694,20 +690,20 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>19/06/2019</t>
+          <t>21/06/2022</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>23/08/2019</t>
+          <t>26/06/2022</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>CAVITAÇÃO</t>
+          <t>(1) PARADA DA ILHA - TRANSFORMADOR (2) MANUTENÇÃO NO CDG</t>
         </is>
       </c>
       <c r="F10" t="inlineStr"/>
@@ -716,25 +712,25 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>ROUHSN_13P8_UG03</t>
+          <t>ROUHSN_13P8_UG04</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>27/09/2019</t>
+          <t>05/10/2021</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>02/10/2019</t>
+          <t>28/11/2021</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>6</v>
+        <v>55</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>(1) PARADA DA ILHA - TRANSFORMADOR (2) MANUTENÇÃO NO CDG</t>
+          <t>(1) MANUTENÇÃO CORRETIVA COMPORTA VAGÃO (2) PARADA DA ILHA - TRANSFORMADOR (3) MANUTENÇÃO NO CDG</t>
         </is>
       </c>
       <c r="F11" t="inlineStr"/>
@@ -748,20 +744,20 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>16/06/2019</t>
+          <t>24/12/2021</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>17/07/2019</t>
+          <t>28/01/2022</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>(1) BIELISMO ROTOR KAPLAN (2) ALTERAÇÃO DA PLATAFORMA DO ARO CÂMARA</t>
+          <t>MANUTENÇÃO CORRETIVA VEDAÇÃO DO EIXO</t>
         </is>
       </c>
       <c r="F12" t="inlineStr"/>
@@ -775,20 +771,20 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>21/07/2019</t>
+          <t>27/06/2022</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>25/08/2019</t>
+          <t>28/07/2022</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>MANUTENÇÃO CORRETIVA VEDAÇÃO DO EIXO</t>
+          <t>(1) BIELISMO ROTOR KAPLAN (2) ALTERAÇÃO DA PLATAFORMA DO ARO CÂMARA</t>
         </is>
       </c>
       <c r="F13" t="inlineStr"/>
@@ -797,25 +793,25 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>ROUHSN_13P8_UG04</t>
+          <t>ROUHSN_13P8_UG05</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>21/09/2019</t>
+          <t>20/08/2021</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>14/11/2019</t>
+          <t>09/09/2021</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>55</v>
+        <v>21</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>(1) MANUTENÇÃO CORRETIVA COMPORTA VAGÃO (2) PARADA DA ILHA - TRANSFORMADOR (3) MANUTENÇÃO NO CDG</t>
+          <t>(1) BIELISMO ROTOR KAPLAN (2) ALTERAÇÃO DA PLATAFORMA DO ARO CÂMARA</t>
         </is>
       </c>
       <c r="F14" t="inlineStr"/>
@@ -829,20 +825,20 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>04/07/2019</t>
+          <t>11/09/2021</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>24/07/2019</t>
+          <t>16/09/2021</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>(1) BIELISMO ROTOR KAPLAN (2) ALTERAÇÃO DA PLATAFORMA DO ARO CÂMARA</t>
+          <t>SUBSTITUIÇÃO VÁLVULA ESVAZIAMENTO UG</t>
         </is>
       </c>
       <c r="F15" t="inlineStr"/>
@@ -856,12 +852,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>07/08/2019</t>
+          <t>11/09/2021</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>12/08/2019</t>
+          <t>16/09/2021</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -869,7 +865,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>SUBSTITUIÇÃO VÁLVULA ESVAZIAMENTO UG</t>
+          <t>(1) PARADA DA ILHA - TRANSFORMADOR (2) MANUTENÇÃO NO CDG</t>
         </is>
       </c>
       <c r="F16" t="inlineStr"/>
@@ -883,12 +879,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>07/08/2019</t>
+          <t>24/09/2021</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>12/08/2019</t>
+          <t>29/09/2021</t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -896,7 +892,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>(1) PARADA DA ILHA - TRANSFORMADOR (2) MANUTENÇÃO NO CDG</t>
+          <t>SUBSTITUIÇÃO VÁLVULA ESVAZIAMENTO UG</t>
         </is>
       </c>
       <c r="F17" t="inlineStr"/>
@@ -910,12 +906,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>10/10/2019</t>
+          <t>24/09/2021</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>15/10/2019</t>
+          <t>29/09/2021</t>
         </is>
       </c>
       <c r="D18" t="n">
@@ -923,7 +919,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>SUBSTITUIÇÃO VÁLVULA ESVAZIAMENTO UG</t>
+          <t>(1) PARADA DA ILHA - TRANSFORMADOR (2) MANUTENÇÃO NO CDG</t>
         </is>
       </c>
       <c r="F18" t="inlineStr"/>
@@ -932,25 +928,25 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>ROUHSN_13P8_UG05</t>
+          <t>ROUHSN_13P8_UG06</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>10/10/2019</t>
+          <t>19/09/2021</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>15/10/2019</t>
+          <t>02/10/2021</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>(1) PARADA DA ILHA - TRANSFORMADOR (2) MANUTENÇÃO NO CDG</t>
+          <t>(1) BIELISMO ROTOR KAPLAN (2) PARADA DA ILHA - TRANSFORMADOR (3) MANUTENÇÃO NO CDG</t>
         </is>
       </c>
       <c r="F19" t="inlineStr"/>
@@ -964,20 +960,20 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>20/07/2019</t>
+          <t>22/12/2021</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>02/08/2019</t>
+          <t>07/01/2022</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>(1) BIELISMO ROTOR KAPLAN (2) PARADA DA ILHA - TRANSFORMADOR (3) MANUTENÇÃO NO CDG</t>
+          <t xml:space="preserve">REFORÇO ARO CAMARA </t>
         </is>
       </c>
       <c r="F20" t="inlineStr"/>
@@ -991,12 +987,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>13/09/2019</t>
+          <t>22/12/2021</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>29/09/2019</t>
+          <t>07/01/2022</t>
         </is>
       </c>
       <c r="D21" t="n">
@@ -1004,7 +1000,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t xml:space="preserve">REFORÇO ARO CAMARA </t>
+          <t>MANUTENÇÃO CORRETIVA COMPORTA VAGÃO</t>
         </is>
       </c>
       <c r="F21" t="inlineStr"/>
@@ -1018,12 +1014,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>13/09/2019</t>
+          <t>12/07/2022</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>29/09/2019</t>
+          <t>28/07/2022</t>
         </is>
       </c>
       <c r="D22" t="n">
@@ -1031,7 +1027,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>MANUTENÇÃO CORRETIVA COMPORTA VAGÃO</t>
+          <t xml:space="preserve">REFORÇO ARO CAMARA </t>
         </is>
       </c>
       <c r="F22" t="inlineStr"/>
@@ -1045,12 +1041,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>17/10/2019</t>
+          <t>12/07/2022</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>02/11/2019</t>
+          <t>28/07/2022</t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -1058,7 +1054,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t xml:space="preserve">REFORÇO ARO CAMARA </t>
+          <t>MANUTENÇÃO CORRETIVA COMPORTA VAGÃO</t>
         </is>
       </c>
       <c r="F23" t="inlineStr"/>
@@ -1067,25 +1063,25 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>ROUHSN_13P8_UG06</t>
+          <t>ROUHSN_13P8_UG07</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>17/10/2019</t>
+          <t>09/08/2021</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>02/11/2019</t>
+          <t>14/08/2021</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>MANUTENÇÃO CORRETIVA COMPORTA VAGÃO</t>
+          <t>(1) PARADA DA ILHA - TRANSFORMADOR (2) MANUTENÇÃO NO CDG</t>
         </is>
       </c>
       <c r="F24" t="inlineStr"/>
@@ -1099,20 +1095,20 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>14/06/2019</t>
+          <t>09/08/2021</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>23/06/2019</t>
+          <t>14/08/2021</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>MANUTENÇÃO CORRETIVA CABEÇOTE KAPLAN</t>
+          <t>RECOMISSIONAMENTO REGULADORES</t>
         </is>
       </c>
       <c r="F25" t="inlineStr"/>
@@ -1126,12 +1122,12 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>11/08/2019</t>
+          <t>16/11/2021</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>16/08/2019</t>
+          <t>21/11/2021</t>
         </is>
       </c>
       <c r="D26" t="n">
@@ -1153,12 +1149,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>11/08/2019</t>
+          <t>16/11/2021</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>16/08/2019</t>
+          <t>21/11/2021</t>
         </is>
       </c>
       <c r="D27" t="n">
@@ -1180,20 +1176,20 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>23/08/2019</t>
+          <t>10/06/2022</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>28/08/2019</t>
+          <t>19/06/2022</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>(1) PARADA DA ILHA - TRANSFORMADOR (2) MANUTENÇÃO NO CDG</t>
+          <t>MANUTENÇÃO CORRETIVA CABEÇOTE KAPLAN</t>
         </is>
       </c>
       <c r="F28" t="inlineStr"/>
@@ -1202,25 +1198,25 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>ROUHSN_13P8_UG07</t>
+          <t>ROUHSN_13P8_UG08</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>23/08/2019</t>
+          <t>28/08/2021</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>28/08/2019</t>
+          <t>16/09/2021</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>RECOMISSIONAMENTO REGULADORES</t>
+          <t>BIELISMO ROTOR KAPLAN</t>
         </is>
       </c>
       <c r="F29" t="inlineStr"/>
@@ -1234,12 +1230,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>23/07/2019</t>
+          <t>24/11/2021</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>23/09/2019</t>
+          <t>25/01/2022</t>
         </is>
       </c>
       <c r="D30" t="n">
@@ -1256,25 +1252,25 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>ROUHSN_13P8_UG08</t>
+          <t>ROUHSN_13P8_UG09</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>13/10/2019</t>
+          <t>08/08/2021</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>01/11/2019</t>
+          <t>25/08/2021</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>BIELISMO ROTOR KAPLAN</t>
+          <t>MANUTENÇÃO CORRETIVA TUBULAÇÃO KAPLAN</t>
         </is>
       </c>
       <c r="F31" t="inlineStr"/>
@@ -1288,18 +1284,22 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>12/07/2019</t>
+          <t>08/08/2021</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>20/08/2019</t>
+          <t>25/08/2021</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>40</v>
-      </c>
-      <c r="E32" t="inlineStr"/>
+        <v>18</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>INSPEÇÃO DAS GRADES DE TOMADA D'ÁGUA</t>
+        </is>
+      </c>
       <c r="F32" t="inlineStr"/>
       <c r="G32" t="inlineStr"/>
     </row>
@@ -1311,20 +1311,20 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>11/09/2019</t>
+          <t>07/07/2022</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>04/11/2019</t>
+          <t>24/07/2022</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>55</v>
+        <v>18</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>(1) MANUTENÇÃO CORRETIVA TUBULAÇÃO KAPLAN + (2) REVISÃO 25000 H (3) BIELISMO ROTOR KAPLAN</t>
+          <t>MANUTENÇÃO CORRETIVA TUBULAÇÃO KAPLAN</t>
         </is>
       </c>
       <c r="F33" t="inlineStr"/>
@@ -1338,12 +1338,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>13/12/2019</t>
+          <t>07/07/2022</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>30/12/2019</t>
+          <t>24/07/2022</t>
         </is>
       </c>
       <c r="D34" t="n">
@@ -1351,7 +1351,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>MANUTENÇÃO CORRETIVA TUBULAÇÃO KAPLAN</t>
+          <t>INSPEÇÃO DAS GRADES DE TOMADA D'ÁGUA</t>
         </is>
       </c>
       <c r="F34" t="inlineStr"/>
@@ -1365,20 +1365,20 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>13/12/2019</t>
+          <t>02/10/2021</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>30/12/2019</t>
+          <t>25/11/2021</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>18</v>
+        <v>55</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>INSPEÇÃO DAS GRADES DE TOMADA D'ÁGUA</t>
+          <t>(1) MANUTENÇÃO CORRETIVA TUBULAÇÃO KAPLAN + (2) REVISÃO 25000 H (3) BIELISMO ROTOR KAPLAN</t>
         </is>
       </c>
       <c r="F35" t="inlineStr"/>
@@ -1387,25 +1387,25 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>ROUHSN_13P8_UG10</t>
+          <t>ROUHSN_13P8_UG09</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>13/06/2019</t>
+          <t>11/12/2021</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>20/07/2019</t>
+          <t>02/01/2022</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>REVISÃO 25000 H</t>
+          <t>INSPEÇÃO NOS MANCIAS</t>
         </is>
       </c>
       <c r="F36" t="inlineStr"/>
@@ -1419,12 +1419,12 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>04/08/2019</t>
+          <t>16/08/2021</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>21/08/2019</t>
+          <t>02/09/2021</t>
         </is>
       </c>
       <c r="D37" t="n">
@@ -1446,20 +1446,20 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>25/09/2019</t>
+          <t>10/10/2021</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>27/09/2019</t>
+          <t>16/11/2021</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>ENSAIO DE RENDIMENTO</t>
+          <t>REVISÃO 25000 H</t>
         </is>
       </c>
       <c r="F38" t="inlineStr"/>
@@ -1468,25 +1468,25 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>ROUHSN_13P8_UG11</t>
+          <t>ROUHSN_13P8_UG10</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>29/06/2019</t>
+          <t>23/07/2022</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>28/07/2019</t>
+          <t>25/07/2022</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>REVISÃO 25000 H</t>
+          <t>ENSAIO DE RENDIMENTO</t>
         </is>
       </c>
       <c r="F39" t="inlineStr"/>
@@ -1500,20 +1500,20 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>31/07/2019</t>
+          <t>06/09/2021</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>13/08/2019</t>
+          <t>15/09/2021</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>BIELISMO ROTOR KAPLAN</t>
+          <t>SUBSTITUIÇÃO VEDAÇÃO MUNHÕES PALHETAS</t>
         </is>
       </c>
       <c r="F40" t="inlineStr"/>
@@ -1527,20 +1527,20 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>01/09/2019</t>
+          <t>25/09/2021</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>10/09/2019</t>
+          <t>22/11/2021</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>10</v>
+        <v>59</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>SUBSTITUIÇÃO VEDAÇÃO MUNHÕES PALHETAS</t>
+          <t>(1) CAVITAÇÃO + (2) REFORÇO ARO CAMARA (3) ALTERAÇÃO DA PLATAFORMA DO ARO CÂMARA</t>
         </is>
       </c>
       <c r="F41" t="inlineStr"/>
@@ -1554,20 +1554,20 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>26/09/2019</t>
+          <t>28/11/2021</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>23/11/2019</t>
+          <t>27/12/2021</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>59</v>
+        <v>30</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>(1) CAVITAÇÃO + (2) REFORÇO ARO CAMARA (3) ALTERAÇÃO DA PLATAFORMA DO ARO CÂMARA</t>
+          <t>REVISÃO 25000 H</t>
         </is>
       </c>
       <c r="F42" t="inlineStr"/>
@@ -1576,25 +1576,25 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>ROUHSN_13P8_UG12</t>
+          <t>ROUHSN_13P8_UG11</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>29/06/2019</t>
+          <t>01/07/2022</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>30/07/2019</t>
+          <t>14/07/2022</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>REVISÃO 25000 H</t>
+          <t>BIELISMO ROTOR KAPLAN</t>
         </is>
       </c>
       <c r="F43" t="inlineStr"/>
@@ -1608,12 +1608,12 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>09/09/2019</t>
+          <t>09/08/2021</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>06/10/2019</t>
+          <t>05/09/2021</t>
         </is>
       </c>
       <c r="D44" t="n">
@@ -1630,21 +1630,21 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>ROUHSN_13P8_UG13</t>
+          <t>ROUHSN_13P8_UG12</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>12/06/2019</t>
+          <t>25/10/2021</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>26/07/2019</t>
+          <t>25/11/2021</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -1662,20 +1662,20 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>28/08/2019</t>
+          <t>15/08/2021</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>30/08/2019</t>
+          <t>28/09/2021</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>ENSAIO DE RENDIMENTO</t>
+          <t>REVISÃO 25000 H</t>
         </is>
       </c>
       <c r="F46" t="inlineStr"/>
@@ -1689,20 +1689,20 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>03/09/2019</t>
+          <t>12/10/2021</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>01/10/2019</t>
+          <t>15/11/2021</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>JUNTA DESLIZANTE</t>
+          <t>ANEL DE REGULAÇÃO</t>
         </is>
       </c>
       <c r="F47" t="inlineStr"/>
@@ -1716,20 +1716,20 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>10/10/2019</t>
+          <t>30/12/2021</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>13/11/2019</t>
+          <t>27/01/2022</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>ANEL DE REGULAÇÃO</t>
+          <t>JUNTA DESLIZANTE</t>
         </is>
       </c>
       <c r="F48" t="inlineStr"/>
@@ -1738,25 +1738,25 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>ROUHSN_13P8_UG14</t>
+          <t>ROUHSN_13P8_UG13</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>12/08/2019</t>
+          <t>05/06/2022</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>15/08/2019</t>
+          <t>07/06/2022</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>RETORNO DE RESTRIÇÃO HIDRICA</t>
+          <t>ENSAIO DE RENDIMENTO</t>
         </is>
       </c>
       <c r="F49" t="inlineStr"/>
@@ -1770,20 +1770,20 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>25/10/2019</t>
+          <t>02/08/2021</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>16/12/2019</t>
+          <t>05/08/2021</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>53</v>
+        <v>4</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>MANUTENÇÃO COMPORTA VAGÃO</t>
+          <t>RETORNO DE RESTRIÇÃO HIDRICA</t>
         </is>
       </c>
       <c r="F50" t="inlineStr"/>
@@ -1792,25 +1792,25 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>ROUHSN_13P8_UG15</t>
+          <t>ROUHSN_13P8_UG14</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>09/09/2019</t>
+          <t>09/09/2021</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>16/10/2019</t>
+          <t>31/10/2021</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>(1) VEDAÇÃO DO EIXO (ILHA 01) (2) SUBSTITUIÇÃO VEDAÇÃO MUNHÕES PALHETAS</t>
+          <t>MANUTENÇÃO COMPORTA VAGÃO</t>
         </is>
       </c>
       <c r="F51" t="inlineStr"/>
@@ -1824,20 +1824,20 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>05/12/2019</t>
+          <t>19/10/2021</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>19/12/2019</t>
+          <t>25/11/2021</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>INSPEÇÃO E MANUTENÇÃO DAS VALVULAS DRENAGEM</t>
+          <t>(1) VEDAÇÃO DO EIXO (ILHA 01) (2) SUBSTITUIÇÃO VEDAÇÃO MUNHÕES PALHETAS</t>
         </is>
       </c>
       <c r="F52" t="inlineStr"/>
@@ -1846,25 +1846,25 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>ROUHSN_13P8_UG17</t>
+          <t>ROUHSN_13P8_UG15</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>20/06/2019</t>
+          <t>06/06/2022</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>30/07/2019</t>
+          <t>20/06/2022</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>VEDAÇÃO DO EIXO</t>
+          <t>INSPEÇÃO E MANUTENÇÃO DAS VALVULAS DRENAGEM</t>
         </is>
       </c>
       <c r="F53" t="inlineStr"/>
@@ -1878,12 +1878,12 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>08/09/2019</t>
+          <t>25/08/2021</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>26/10/2019</t>
+          <t>12/10/2021</t>
         </is>
       </c>
       <c r="D54" t="n">
@@ -1900,25 +1900,25 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>ROUHSN_13P8_UG18</t>
+          <t>ROUHSN_13P8_UG17</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>06/08/2019</t>
+          <t>19/10/2021</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>07/09/2019</t>
+          <t>28/11/2021</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>VEDAÇÃO DO EIXO (ILHA 01)</t>
+          <t>VEDAÇÃO DO EIXO</t>
         </is>
       </c>
       <c r="F55" t="inlineStr"/>
@@ -1927,25 +1927,25 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>ROUHSN_13P8_UG20</t>
+          <t>ROUHSN_13P8_UG18</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>27/06/2019</t>
+          <t>18/10/2021</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>21/07/2019</t>
+          <t>19/11/2021</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>VEDAÇÃO DO EIXO (ILHA 02)</t>
+          <t>VEDAÇÃO DO EIXO (ILHA 01)</t>
         </is>
       </c>
       <c r="F56" t="inlineStr"/>
@@ -1959,20 +1959,20 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>27/08/2019</t>
+          <t>22/08/2021</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>17/09/2019</t>
+          <t>14/09/2021</t>
         </is>
       </c>
       <c r="D57" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>MANUTENÇÃO CORRETIVA SISTEMA REG VEL</t>
+          <t>SUBSTITUIÇÃO VEDAÇÃO MUNHÕES PALHETAS</t>
         </is>
       </c>
       <c r="F57" t="inlineStr"/>
@@ -1986,20 +1986,20 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>19/09/2019</t>
+          <t>02/10/2021</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>12/10/2019</t>
+          <t>23/10/2021</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>SUBSTITUIÇÃO VEDAÇÃO MUNHÕES PALHETAS</t>
+          <t>MANUTENÇÃO CORRETIVA SISTEMA REG VEL</t>
         </is>
       </c>
       <c r="F58" t="inlineStr"/>
@@ -2008,25 +2008,25 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>ROUHSN_13P8_UG21</t>
+          <t>ROUHSN_13P8_UG20</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>22/08/2019</t>
+          <t>12/06/2022</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>09/09/2019</t>
+          <t>06/07/2022</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>PERITAGEM DO ROTOR KAPLAN</t>
+          <t>VEDAÇÃO DO EIXO (ILHA 02)</t>
         </is>
       </c>
       <c r="F59" t="inlineStr"/>
@@ -2040,20 +2040,20 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>05/10/2019</t>
+          <t>26/09/2021</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>10/10/2019</t>
+          <t>14/10/2021</t>
         </is>
       </c>
       <c r="D60" t="n">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>PARADA DA ILHA - TRANSFORMADOR</t>
+          <t>PERITAGEM DO ROTOR KAPLAN</t>
         </is>
       </c>
       <c r="F60" t="inlineStr"/>
@@ -2062,25 +2062,25 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>ROUHSN_13P8_UG22</t>
+          <t>ROUHSN_13P8_UG21</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>02/06/2019</t>
+          <t>16/11/2021</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>05/07/2019</t>
+          <t>21/11/2021</t>
         </is>
       </c>
       <c r="D61" t="n">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>(1) REVISÃO 25000 H (2) MANUTENÇÃO CORRETIVA VEDAÇÃO DO EIXO</t>
+          <t>PARADA DA ILHA - TRANSFORMADOR</t>
         </is>
       </c>
       <c r="F61" t="inlineStr"/>
@@ -2094,22 +2094,18 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>28/07/2019</t>
+          <t>02/08/2021</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>01/08/2019</t>
+          <t>22/08/2021</t>
         </is>
       </c>
       <c r="D62" t="n">
-        <v>5</v>
-      </c>
-      <c r="E62" t="inlineStr">
-        <is>
-          <t>ALTERAÇÃO DA PLATAFORMA DO ARO CÂMARA</t>
-        </is>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="E62" t="inlineStr"/>
       <c r="F62" t="inlineStr"/>
       <c r="G62" t="inlineStr"/>
     </row>
@@ -2121,20 +2117,20 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>08/08/2019</t>
+          <t>25/08/2021</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>31/08/2019</t>
+          <t>27/09/2021</t>
         </is>
       </c>
       <c r="D63" t="n">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>MANUTENÇÃO CORRETIVA VEDAÇÃO DO EIXO</t>
+          <t>(1) REVISÃO 25000 H (2) MANUTENÇÃO CORRETIVA VEDAÇÃO DO EIXO</t>
         </is>
       </c>
       <c r="F63" t="inlineStr"/>
@@ -2148,20 +2144,20 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>09/09/2019</t>
+          <t>17/10/2021</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>27/09/2019</t>
+          <t>22/10/2021</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>BIELISMO ROTOR KAPLAN</t>
+          <t>PARADA DA ILHA - TRANSFORMADOR</t>
         </is>
       </c>
       <c r="F64" t="inlineStr"/>
@@ -2175,18 +2171,22 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>06/10/2019</t>
+          <t>28/10/2021</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>20/11/2019</t>
+          <t>07/12/2021</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>46</v>
-      </c>
-      <c r="E65" t="inlineStr"/>
+        <v>41</v>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>MANUTENÇÃO CORRETIVA VEDAÇÃO DO EIXO</t>
+        </is>
+      </c>
       <c r="F65" t="inlineStr"/>
       <c r="G65" t="inlineStr"/>
     </row>
@@ -2198,20 +2198,20 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>02/12/2019</t>
+          <t>21/12/2021</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>04/12/2019</t>
+          <t>25/12/2021</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>ENSAIO DE RENDIMENTO</t>
+          <t>ALTERAÇÃO DA PLATAFORMA DO ARO CÂMARA</t>
         </is>
       </c>
       <c r="F66" t="inlineStr"/>
@@ -2225,20 +2225,20 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>07/12/2019</t>
+          <t>01/01/2022</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>28/12/2019</t>
+          <t>24/01/2022</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>VEDAÇÃO DO EIXO</t>
+          <t>MANUTENÇÃO CORRETIVA VEDAÇÃO DO EIXO</t>
         </is>
       </c>
       <c r="F67" t="inlineStr"/>
@@ -2247,25 +2247,25 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>ROUHSN_13P8_UG23</t>
+          <t>ROUHSN_13P8_UG22</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>30/08/2019</t>
+          <t>04/07/2022</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>04/09/2019</t>
+          <t>25/07/2022</t>
         </is>
       </c>
       <c r="D68" t="n">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>(1) PARADA DA ILHA - TRANSFORMADOR (2) MANUTENÇÃO NO CDG</t>
+          <t>VEDAÇÃO DO EIXO</t>
         </is>
       </c>
       <c r="F68" t="inlineStr"/>
@@ -2279,12 +2279,12 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>18/09/2019</t>
+          <t>02/08/2021</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>16/10/2019</t>
+          <t>30/08/2021</t>
         </is>
       </c>
       <c r="D69" t="n">
@@ -2301,25 +2301,25 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>ROUHSN_13P8_UG24</t>
+          <t>ROUHSN_13P8_UG23</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>03/06/2019</t>
+          <t>21/10/2021</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>04/07/2019</t>
+          <t>26/10/2021</t>
         </is>
       </c>
       <c r="D70" t="n">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>CORREÇÃO DE VAZAMENTO ROTOR KAPLAN</t>
+          <t>(1) PARADA DA ILHA - TRANSFORMADOR (2) MANUTENÇÃO NO CDG</t>
         </is>
       </c>
       <c r="F70" t="inlineStr"/>
@@ -2333,12 +2333,12 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>09/07/2019</t>
+          <t>09/08/2021</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>14/07/2019</t>
+          <t>14/08/2021</t>
         </is>
       </c>
       <c r="D71" t="n">
@@ -2360,12 +2360,12 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>09/07/2019</t>
+          <t>09/08/2021</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>14/07/2019</t>
+          <t>14/08/2021</t>
         </is>
       </c>
       <c r="D72" t="n">
@@ -2387,12 +2387,12 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>23/09/2019</t>
+          <t>26/10/2021</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>28/09/2019</t>
+          <t>31/10/2021</t>
         </is>
       </c>
       <c r="D73" t="n">
@@ -2414,12 +2414,12 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>23/09/2019</t>
+          <t>26/10/2021</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>28/09/2019</t>
+          <t>31/10/2021</t>
         </is>
       </c>
       <c r="D74" t="n">
@@ -2441,20 +2441,20 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>10/10/2019</t>
+          <t>27/08/2021</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>01/11/2019</t>
+          <t>27/09/2021</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t xml:space="preserve">VEDAÇÃO DO EIXO </t>
+          <t>CORREÇÃO DE VAZAMENTO ROTOR KAPLAN</t>
         </is>
       </c>
       <c r="F75" t="inlineStr"/>
@@ -2463,25 +2463,25 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>ROUHSN_13P8_UG25</t>
+          <t>ROUHSN_13P8_UG24</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>19/06/2019</t>
+          <t>01/10/2021</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>31/08/2019</t>
+          <t>23/10/2021</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>74</v>
+        <v>23</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>(1) REVISÃO 25000 H (2) ANEL DE REGULAÇÃO + (3) JUNTA DESLIZANTE</t>
+          <t xml:space="preserve">VEDAÇÃO DO EIXO </t>
         </is>
       </c>
       <c r="F76" t="inlineStr"/>
@@ -2490,25 +2490,25 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>ROUHSN_13P8_UG26</t>
+          <t>ROUHSN_13P8_UG25</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>11/07/2019</t>
+          <t>31/08/2021</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>25/08/2019</t>
+          <t>12/11/2021</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>46</v>
+        <v>74</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>JUNTA DESLIZANTE</t>
+          <t>(1) REVISÃO 25000 H (2) ANEL DE REGULAÇÃO + (3) JUNTA DESLIZANTE</t>
         </is>
       </c>
       <c r="F77" t="inlineStr"/>
@@ -2522,20 +2522,20 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>27/08/2019</t>
+          <t>15/08/2021</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>29/08/2019</t>
+          <t>01/09/2021</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>ENSAIO DE RENDIMENTO</t>
+          <t>VEDAÇÃO DO EIXO (ILHA 01)</t>
         </is>
       </c>
       <c r="F78" t="inlineStr"/>
@@ -2549,20 +2549,20 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>01/09/2019</t>
+          <t>20/11/2021</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>18/09/2019</t>
+          <t>22/11/2021</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>VEDAÇÃO DO EIXO (ILHA 01)</t>
+          <t>ENSAIO DE RENDIMENTO</t>
         </is>
       </c>
       <c r="F79" t="inlineStr"/>
@@ -2571,25 +2571,25 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>ROUHSN_13P8_UG27</t>
+          <t>ROUHSN_13P8_UG26</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>13/06/2019</t>
+          <t>01/06/2022</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>12/07/2019</t>
+          <t>16/07/2022</t>
         </is>
       </c>
       <c r="D80" t="n">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>SUBSTITUIÇÃO VEDAÇÃO MUNHÕES PALHETAS</t>
+          <t>JUNTA DESLIZANTE</t>
         </is>
       </c>
       <c r="F80" t="inlineStr"/>
@@ -2603,20 +2603,20 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>31/08/2019</t>
+          <t>12/08/2021</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>13/09/2019</t>
+          <t>22/09/2021</t>
         </is>
       </c>
       <c r="D81" t="n">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>MANUTENÇÃO CORRETIVA VEDAÇÃO DO EIXO</t>
+          <t>(1) REVISÃO 25000 H (2) ANEL DE REGULAÇÃO (3) MAPEAMENTO 3D ROTOR KAPLAN (4) LUBRIFICAÇÃO CENTRALIZADA</t>
         </is>
       </c>
       <c r="F81" t="inlineStr"/>
@@ -2630,20 +2630,20 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>22/09/2019</t>
+          <t>07/10/2021</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>02/11/2019</t>
+          <t>05/11/2021</t>
         </is>
       </c>
       <c r="D82" t="n">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>(1) REVISÃO 25000 H (2) ANEL DE REGULAÇÃO (3) MAPEAMENTO 3D ROTOR KAPLAN (4) LUBRIFICAÇÃO CENTRALIZADA</t>
+          <t>SUBSTITUIÇÃO VEDAÇÃO MUNHÕES PALHETAS</t>
         </is>
       </c>
       <c r="F82" t="inlineStr"/>
@@ -2652,25 +2652,25 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>ROUHSN_13P8_UG28</t>
+          <t>ROUHSN_13P8_UG27</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>07/10/2019</t>
+          <t>28/11/2021</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>04/11/2019</t>
+          <t>11/12/2021</t>
         </is>
       </c>
       <c r="D83" t="n">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>VEDAÇÃO DO EIXO</t>
+          <t>MANUTENÇÃO CORRETIVA VEDAÇÃO DO EIXO</t>
         </is>
       </c>
       <c r="F83" t="inlineStr"/>
@@ -2679,25 +2679,25 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>ROUHSN_13P8_UG29</t>
+          <t>ROUHSN_13P8_UG28</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>08/08/2019</t>
+          <t>22/08/2021</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>03/09/2019</t>
+          <t>19/09/2021</t>
         </is>
       </c>
       <c r="D84" t="n">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>SUBSTITUIÇÃO DE TRUG</t>
+          <t>VEDAÇÃO DO EIXO</t>
         </is>
       </c>
       <c r="F84" t="inlineStr"/>
@@ -2711,22 +2711,18 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>26/11/2019</t>
+          <t>07/08/2021</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>26/12/2019</t>
+          <t>03/10/2021</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>31</v>
-      </c>
-      <c r="E85" t="inlineStr">
-        <is>
-          <t>VEDAÇÃO DO EIXO</t>
-        </is>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="E85" t="inlineStr"/>
       <c r="F85" t="inlineStr"/>
       <c r="G85" t="inlineStr"/>
     </row>
@@ -2738,20 +2734,20 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>08/06/2019</t>
+          <t>13/08/2021</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>26/06/2019</t>
+          <t>07/09/2021</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>MANUTENÇÃO CORRETIVA VEDAÇÃO DO EIXO</t>
+          <t>JUNTA DESLIZANTE</t>
         </is>
       </c>
       <c r="F86" t="inlineStr"/>
@@ -2765,20 +2761,20 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>06/08/2019</t>
+          <t>09/09/2021</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>01/09/2019</t>
+          <t>27/09/2021</t>
         </is>
       </c>
       <c r="D87" t="n">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>SUBSTITUIÇÃO DE TRUG</t>
+          <t>MANUTENÇÃO CORRETIVA VEDAÇÃO DO EIXO</t>
         </is>
       </c>
       <c r="F87" t="inlineStr"/>
@@ -2792,12 +2788,12 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>09/09/2019</t>
+          <t>09/10/2021</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>02/10/2019</t>
+          <t>01/11/2021</t>
         </is>
       </c>
       <c r="D88" t="n">
@@ -2819,20 +2815,20 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>19/11/2019</t>
+          <t>08/06/2022</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>14/12/2019</t>
+          <t>04/07/2022</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>JUNTA DESLIZANTE</t>
+          <t>SUBSTITUIÇÃO DE TRUG</t>
         </is>
       </c>
       <c r="F89" t="inlineStr"/>
@@ -2846,20 +2842,20 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>14/07/2019</t>
+          <t>20/09/2021</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>04/08/2019</t>
+          <t>07/10/2021</t>
         </is>
       </c>
       <c r="D90" t="n">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>VEDAÇÃO DO EIXO</t>
+          <t>BIELISMO ROTOR KAPLAN</t>
         </is>
       </c>
       <c r="F90" t="inlineStr"/>
@@ -2873,20 +2869,20 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>04/09/2019</t>
+          <t>02/12/2021</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>21/09/2019</t>
+          <t>28/12/2021</t>
         </is>
       </c>
       <c r="D91" t="n">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>BIELISMO ROTOR KAPLAN</t>
+          <t>SUBSTITUIÇÃO DE TRUG</t>
         </is>
       </c>
       <c r="F91" t="inlineStr"/>
@@ -2900,20 +2896,20 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>02/10/2019</t>
+          <t>07/07/2022</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>28/10/2019</t>
+          <t>28/07/2022</t>
         </is>
       </c>
       <c r="D92" t="n">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>SUBSTITUIÇÃO DE TRUG</t>
+          <t>VEDAÇÃO DO EIXO</t>
         </is>
       </c>
       <c r="F92" t="inlineStr"/>
@@ -2927,20 +2923,20 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>13/06/2019</t>
+          <t>21/08/2021</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>10/08/2019</t>
+          <t>16/09/2021</t>
         </is>
       </c>
       <c r="D93" t="n">
-        <v>59</v>
+        <v>27</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>CAVITAÇÃO</t>
+          <t>SUBSTITUIÇÃO DE TRUG</t>
         </is>
       </c>
       <c r="F93" t="inlineStr"/>
@@ -2954,12 +2950,12 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>20/08/2019</t>
+          <t>24/09/2021</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>09/09/2019</t>
+          <t>14/10/2021</t>
         </is>
       </c>
       <c r="D94" t="n">
@@ -2981,20 +2977,20 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>13/09/2019</t>
+          <t>14/11/2021</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>29/09/2019</t>
+          <t>11/01/2022</t>
         </is>
       </c>
       <c r="D95" t="n">
-        <v>17</v>
+        <v>59</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>(1) BIELISMO ROTOR KAPLAN (2) ALTERAÇÃO DA PLATAFORMA DO ARO CÂMARA</t>
+          <t>CAVITAÇÃO</t>
         </is>
       </c>
       <c r="F95" t="inlineStr"/>
@@ -3008,20 +3004,20 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>20/11/2019</t>
+          <t>14/07/2022</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>16/12/2019</t>
+          <t>30/07/2022</t>
         </is>
       </c>
       <c r="D96" t="n">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>SUBSTITUIÇÃO DE TRUG</t>
+          <t>(1) BIELISMO ROTOR KAPLAN (2) ALTERAÇÃO DA PLATAFORMA DO ARO CÂMARA</t>
         </is>
       </c>
       <c r="F96" t="inlineStr"/>
@@ -3035,20 +3031,20 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>20/08/2019</t>
+          <t>11/08/2021</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>26/08/2019</t>
+          <t>16/08/2021</t>
         </is>
       </c>
       <c r="D97" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>PARADA DA ILHA - TRANSFORMADOR</t>
+          <t>RECOMISSIONAMENTO REGULADORES</t>
         </is>
       </c>
       <c r="F97" t="inlineStr"/>
@@ -3062,20 +3058,20 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>20/09/2019</t>
+          <t>18/09/2021</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>19/10/2019</t>
+          <t>24/09/2021</t>
         </is>
       </c>
       <c r="D98" t="n">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>MANUTENÇÃO CORRETIVA TUBULAÇÃO KAPLAN</t>
+          <t>PARADA DA ILHA - TRANSFORMADOR</t>
         </is>
       </c>
       <c r="F98" t="inlineStr"/>
@@ -3089,20 +3085,20 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>28/10/2019</t>
+          <t>26/09/2021</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>11/11/2019</t>
+          <t>25/10/2021</t>
         </is>
       </c>
       <c r="D99" t="n">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>VEDAÇÃO DO EIXO</t>
+          <t>MANUTENÇÃO CORRETIVA TUBULAÇÃO KAPLAN</t>
         </is>
       </c>
       <c r="F99" t="inlineStr"/>
@@ -3116,20 +3112,20 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>15/11/2019</t>
+          <t>14/07/2022</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>20/11/2019</t>
+          <t>28/07/2022</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>RECOMISSIONAMENTO REGULADORES</t>
+          <t>VEDAÇÃO DO EIXO</t>
         </is>
       </c>
       <c r="F100" t="inlineStr"/>
@@ -3143,12 +3139,12 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>16/07/2019</t>
+          <t>04/08/2021</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>22/07/2019</t>
+          <t>10/08/2021</t>
         </is>
       </c>
       <c r="D101" t="n">
@@ -3170,20 +3166,20 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>18/11/2019</t>
+          <t>24/12/2021</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>13/12/2019</t>
+          <t>26/12/2021</t>
         </is>
       </c>
       <c r="D102" t="n">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>VEDAÇÃO DO EIXO</t>
+          <t>LUBRIFICAÇÃO CENTRALIZADA</t>
         </is>
       </c>
       <c r="F102" t="inlineStr"/>
@@ -3197,20 +3193,20 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>26/12/2019</t>
+          <t>21/06/2022</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>28/12/2019</t>
+          <t>16/07/2022</t>
         </is>
       </c>
       <c r="D103" t="n">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>LUBRIFICAÇÃO CENTRALIZADA</t>
+          <t>VEDAÇÃO DO EIXO</t>
         </is>
       </c>
       <c r="F103" t="inlineStr"/>
@@ -3224,20 +3220,20 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>02/06/2019</t>
+          <t>21/10/2021</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>17/06/2019</t>
+          <t>23/10/2021</t>
         </is>
       </c>
       <c r="D104" t="n">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>(1) BIELISMO ROTOR KAPLAN + (2) PARADA DA ILHA - TRANSFORMADOR</t>
+          <t>LUBRIFICAÇÃO CENTRALIZADA</t>
         </is>
       </c>
       <c r="F104" t="inlineStr"/>
@@ -3251,20 +3247,20 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>22/11/2019</t>
+          <t>08/06/2022</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>24/11/2019</t>
+          <t>23/06/2022</t>
         </is>
       </c>
       <c r="D105" t="n">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>LUBRIFICAÇÃO CENTRALIZADA</t>
+          <t>(1) BIELISMO ROTOR KAPLAN + (2) PARADA DA ILHA - TRANSFORMADOR</t>
         </is>
       </c>
       <c r="F105" t="inlineStr"/>
@@ -3278,12 +3274,12 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>02/01/2019</t>
+          <t>25/10/2021</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>16/01/2019</t>
+          <t>08/11/2021</t>
         </is>
       </c>
       <c r="D106" t="n">
@@ -3305,12 +3301,12 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>11/04/2019</t>
+          <t>13/11/2021</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>08/07/2019</t>
+          <t>09/02/2022</t>
         </is>
       </c>
       <c r="D107" t="n">
@@ -3332,12 +3328,12 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>16/10/2019</t>
+          <t>14/05/2022</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>09/12/2019</t>
+          <t>07/07/2022</t>
         </is>
       </c>
       <c r="D108" t="n">
@@ -3359,12 +3355,12 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>17/12/2019</t>
+          <t>13/07/2022</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>23/12/2019</t>
+          <t>19/07/2022</t>
         </is>
       </c>
       <c r="D109" t="n">
@@ -3386,12 +3382,12 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>20/07/2019</t>
+          <t>13/10/2021</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>09/08/2019</t>
+          <t>02/11/2021</t>
         </is>
       </c>
       <c r="D110" t="n">
@@ -3413,12 +3409,12 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>27/11/2019</t>
+          <t>05/06/2022</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>25/12/2019</t>
+          <t>03/07/2022</t>
         </is>
       </c>
       <c r="D111" t="n">
@@ -3440,12 +3436,12 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>24/06/2019</t>
+          <t>03/06/2022</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>12/07/2019</t>
+          <t>21/06/2022</t>
         </is>
       </c>
       <c r="D112" t="n">
@@ -3467,12 +3463,12 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>20/11/2019</t>
+          <t>30/06/2022</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>13/12/2019</t>
+          <t>23/07/2022</t>
         </is>
       </c>
       <c r="D113" t="n">
@@ -3494,12 +3490,12 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>29/09/2019</t>
+          <t>08/12/2021</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>16/10/2019</t>
+          <t>25/12/2021</t>
         </is>
       </c>
       <c r="D114" t="n">
@@ -3521,12 +3517,12 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>29/09/2019</t>
+          <t>08/12/2021</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>16/10/2019</t>
+          <t>25/12/2021</t>
         </is>
       </c>
       <c r="D115" t="n">
@@ -3548,12 +3544,12 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>31/10/2019</t>
+          <t>07/06/2022</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>17/11/2019</t>
+          <t>24/06/2022</t>
         </is>
       </c>
       <c r="D116" t="n">
@@ -3575,12 +3571,12 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>31/10/2019</t>
+          <t>07/06/2022</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>17/11/2019</t>
+          <t>24/06/2022</t>
         </is>
       </c>
       <c r="D117" t="n">
@@ -3602,12 +3598,12 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>05/10/2019</t>
+          <t>05/09/2021</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>26/10/2019</t>
+          <t>26/09/2021</t>
         </is>
       </c>
       <c r="D118" t="n">
@@ -3629,20 +3625,20 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>08/06/2019</t>
+          <t>12/08/2021</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>01/07/2019</t>
+          <t>21/09/2021</t>
         </is>
       </c>
       <c r="D119" t="n">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>MANUTENÇÃO CORRETIVA VEDAÇÃO DO EIXO</t>
+          <t>MANUTENÇÃO CORRETIVA SISTEMA REG VEL</t>
         </is>
       </c>
       <c r="F119" t="inlineStr"/>
@@ -3656,20 +3652,20 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>04/08/2019</t>
+          <t>07/10/2021</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>09/08/2019</t>
+          <t>07/11/2021</t>
         </is>
       </c>
       <c r="D120" t="n">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>(1) PARADA DA ILHA - TRANSFORMADOR (2) MANUTENÇÃO NO CDG</t>
+          <t>(1) VEDAÇÃO DO EIXO (ILHA 02) + (2) SUBSTITUIÇÃO VEDAÇÃO MUNHÕES PALHETAS</t>
         </is>
       </c>
       <c r="F120" t="inlineStr"/>
@@ -3683,20 +3679,20 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>24/08/2019</t>
+          <t>21/11/2021</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>03/10/2019</t>
+          <t>14/12/2021</t>
         </is>
       </c>
       <c r="D121" t="n">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>MANUTENÇÃO CORRETIVA SISTEMA REG VEL</t>
+          <t>MANUTENÇÃO CORRETIVA VEDAÇÃO DO EIXO</t>
         </is>
       </c>
       <c r="F121" t="inlineStr"/>
@@ -3710,20 +3706,20 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>23/11/2019</t>
+          <t>24/07/2022</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>24/12/2019</t>
+          <t>29/07/2022</t>
         </is>
       </c>
       <c r="D122" t="n">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>(1) VEDAÇÃO DO EIXO (ILHA 02) + (2) SUBSTITUIÇÃO VEDAÇÃO MUNHÕES PALHETAS</t>
+          <t>(1) PARADA DA ILHA - TRANSFORMADOR (2) MANUTENÇÃO NO CDG</t>
         </is>
       </c>
       <c r="F122" t="inlineStr"/>
@@ -3737,20 +3733,20 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>07/04/2019</t>
+          <t>14/08/2021</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>02/06/2019</t>
+          <t>19/08/2021</t>
         </is>
       </c>
       <c r="D123" t="n">
-        <v>57</v>
+        <v>6</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>MANUTENÇÃO CORRETIVA TUBULAÇÃO KAPLAN</t>
+          <t>(1) PARADA DA ILHA - TRANSFORMADOR (2) MANUTENÇÃO NO CDG</t>
         </is>
       </c>
       <c r="F123" t="inlineStr"/>
@@ -3764,47 +3760,43 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>01/09/2019</t>
+          <t>26/04/2022</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>06/09/2019</t>
+          <t>16/07/2022</t>
         </is>
       </c>
       <c r="D124" t="n">
-        <v>6</v>
-      </c>
-      <c r="E124" t="inlineStr">
-        <is>
-          <t>(1) PARADA DA ILHA - TRANSFORMADOR (2) MANUTENÇÃO NO CDG</t>
-        </is>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="E124" t="inlineStr"/>
       <c r="F124" t="inlineStr"/>
       <c r="G124" t="inlineStr"/>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>ROUHSN_13P8_UG42</t>
+          <t>ROUHSN_13P8_UG43</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>21/11/2019</t>
+          <t>28/08/2021</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>16/12/2019</t>
+          <t>17/09/2021</t>
         </is>
       </c>
       <c r="D125" t="n">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>VEDAÇÃO DO EIXO (ILHA 02)</t>
+          <t>MANUTENÇÃO CORRETIVA VEDAÇÃO DO EIXO</t>
         </is>
       </c>
       <c r="F125" t="inlineStr"/>
@@ -3818,12 +3810,12 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>08/06/2019</t>
+          <t>06/10/2021</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>13/06/2019</t>
+          <t>11/10/2021</t>
         </is>
       </c>
       <c r="D126" t="n">
@@ -3845,12 +3837,12 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>20/07/2019</t>
+          <t>20/07/2022</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>30/07/2019</t>
+          <t>30/07/2022</t>
         </is>
       </c>
       <c r="D127" t="n">
@@ -3867,25 +3859,25 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>ROUHSN_13P8_UG43</t>
+          <t>ROUHSN_13P8_UG44</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>18/09/2019</t>
+          <t>11/08/2021</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>08/10/2019</t>
+          <t>04/09/2021</t>
         </is>
       </c>
       <c r="D128" t="n">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>MANUTENÇÃO CORRETIVA VEDAÇÃO DO EIXO</t>
+          <t>VEDAÇÃO DO EIXO</t>
         </is>
       </c>
       <c r="F128" t="inlineStr"/>
@@ -3899,20 +3891,20 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>09/06/2019</t>
+          <t>18/09/2021</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>25/06/2019</t>
+          <t>23/09/2021</t>
         </is>
       </c>
       <c r="D129" t="n">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>JUNTA DESLIZANTE</t>
+          <t>(1) PARADA DA ILHA - TRANSFORMADOR (2) MANUTENÇÃO NO CDG</t>
         </is>
       </c>
       <c r="F129" t="inlineStr"/>
@@ -3926,20 +3918,20 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>21/09/2019</t>
+          <t>04/10/2021</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>26/09/2019</t>
+          <t>20/10/2021</t>
         </is>
       </c>
       <c r="D130" t="n">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>(1) PARADA DA ILHA - TRANSFORMADOR (2) MANUTENÇÃO NO CDG</t>
+          <t>JUNTA DESLIZANTE</t>
         </is>
       </c>
       <c r="F130" t="inlineStr"/>
@@ -3948,25 +3940,25 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>ROUHSN_13P8_UG44</t>
+          <t>ROUHSN_13P8_UG45</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>15/10/2019</t>
+          <t>22/08/2021</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>08/11/2019</t>
+          <t>09/09/2021</t>
         </is>
       </c>
       <c r="D131" t="n">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>VEDAÇÃO DO EIXO</t>
+          <t>BIELISMO ROTOR KAPLAN</t>
         </is>
       </c>
       <c r="F131" t="inlineStr"/>
@@ -3980,12 +3972,12 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>03/01/2019</t>
+          <t>22/08/2021</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>21/01/2019</t>
+          <t>09/09/2021</t>
         </is>
       </c>
       <c r="D132" t="n">
@@ -3993,7 +3985,7 @@
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>BIELISMO ROTOR KAPLAN</t>
+          <t>MANUTENÇÃO CORRETIVA VEDAÇÃO DO EIXO</t>
         </is>
       </c>
       <c r="F132" t="inlineStr"/>
@@ -4007,12 +3999,12 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>03/01/2019</t>
+          <t>06/10/2021</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>21/01/2019</t>
+          <t>24/10/2021</t>
         </is>
       </c>
       <c r="D133" t="n">
@@ -4020,7 +4012,7 @@
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>MANUTENÇÃO CORRETIVA VEDAÇÃO DO EIXO</t>
+          <t>BIELISMO ROTOR KAPLAN</t>
         </is>
       </c>
       <c r="F133" t="inlineStr"/>
@@ -4034,12 +4026,12 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>02/07/2019</t>
+          <t>06/10/2021</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>20/07/2019</t>
+          <t>24/10/2021</t>
         </is>
       </c>
       <c r="D134" t="n">
@@ -4047,7 +4039,7 @@
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>BIELISMO ROTOR KAPLAN</t>
+          <t>MANUTENÇÃO CORRETIVA VEDAÇÃO DO EIXO</t>
         </is>
       </c>
       <c r="F134" t="inlineStr"/>
@@ -4056,25 +4048,25 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>ROUHSN_13P8_UG45</t>
+          <t>ROUHSN_13P8_UG46</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>02/07/2019</t>
+          <t>14/08/2021</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>20/07/2019</t>
+          <t>16/08/2021</t>
         </is>
       </c>
       <c r="D135" t="n">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>MANUTENÇÃO CORRETIVA VEDAÇÃO DO EIXO</t>
+          <t>RECOMISSIONAMENTO REGULADORES</t>
         </is>
       </c>
       <c r="F135" t="inlineStr"/>
@@ -4088,20 +4080,20 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>05/08/2019</t>
+          <t>24/08/2021</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>07/08/2019</t>
+          <t>10/09/2021</t>
         </is>
       </c>
       <c r="D136" t="n">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>RECOMISSIONAMENTO REGULADORES</t>
+          <t>BIELISMO ROTOR KAPLAN</t>
         </is>
       </c>
       <c r="F136" t="inlineStr"/>
@@ -4115,12 +4107,12 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>21/09/2019</t>
+          <t>02/10/2021</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>30/10/2019</t>
+          <t>10/11/2021</t>
         </is>
       </c>
       <c r="D137" t="n">
@@ -4137,25 +4129,25 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>ROUHSN_13P8_UG46</t>
+          <t>ROUHSN_13P8_UG47</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>26/11/2019</t>
+          <t>21/08/2021</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>13/12/2019</t>
+          <t>08/09/2021</t>
         </is>
       </c>
       <c r="D138" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>BIELISMO ROTOR KAPLAN</t>
+          <t>MANUTENÇÃO CORRETIVA VEDAÇÃO DO EIXO</t>
         </is>
       </c>
       <c r="F138" t="inlineStr"/>
@@ -4169,20 +4161,20 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>04/08/2019</t>
+          <t>15/09/2021</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>22/08/2019</t>
+          <t>02/10/2021</t>
         </is>
       </c>
       <c r="D139" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>MANUTENÇÃO CORRETIVA VEDAÇÃO DO EIXO</t>
+          <t>BIELISMO ROTOR KAPLAN</t>
         </is>
       </c>
       <c r="F139" t="inlineStr"/>
@@ -4196,20 +4188,20 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>17/10/2019</t>
+          <t>06/07/2022</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>03/11/2019</t>
+          <t>11/07/2022</t>
         </is>
       </c>
       <c r="D140" t="n">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>BIELISMO ROTOR KAPLAN</t>
+          <t>RECOMISSIONAMENTO REGULADORES</t>
         </is>
       </c>
       <c r="F140" t="inlineStr"/>
@@ -4218,25 +4210,25 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>ROUHSN_13P8_UG47</t>
+          <t>ROUHSN_13P8_UG48</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>06/11/2019</t>
+          <t>26/08/2021</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>11/11/2019</t>
+          <t>21/11/2021</t>
         </is>
       </c>
       <c r="D141" t="n">
-        <v>6</v>
+        <v>88</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>RECOMISSIONAMENTO REGULADORES</t>
+          <t xml:space="preserve">(1) CAVITAÇÃO (2) REFORÇO ARO CAMARA </t>
         </is>
       </c>
       <c r="F141" t="inlineStr"/>
@@ -4250,12 +4242,12 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>11/07/2019</t>
+          <t>03/01/2022</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>18/07/2019</t>
+          <t>10/01/2022</t>
         </is>
       </c>
       <c r="D142" t="n">
@@ -4277,20 +4269,20 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>01/09/2019</t>
+          <t>01/07/2022</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>27/11/2019</t>
+          <t>15/07/2022</t>
         </is>
       </c>
       <c r="D143" t="n">
-        <v>88</v>
+        <v>15</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t xml:space="preserve">(1) CAVITAÇÃO (2) REFORÇO ARO CAMARA </t>
+          <t>MANUTENÇÃO CORRETIVA VEDAÇÃO DO EIXO</t>
         </is>
       </c>
       <c r="F143" t="inlineStr"/>
@@ -4299,25 +4291,25 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>ROUHSN_13P8_UG48</t>
+          <t>ROUHSN_13P8_UG49</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>09/12/2019</t>
+          <t>05/08/2021</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>23/12/2019</t>
+          <t>25/08/2021</t>
         </is>
       </c>
       <c r="D144" t="n">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>MANUTENÇÃO CORRETIVA VEDAÇÃO DO EIXO</t>
+          <t>VEDAÇÃO DO EIXO</t>
         </is>
       </c>
       <c r="F144" t="inlineStr"/>
@@ -4331,12 +4323,12 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>20/07/2019</t>
+          <t>04/09/2021</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>08/08/2019</t>
+          <t>23/09/2021</t>
         </is>
       </c>
       <c r="D145" t="n">
@@ -4358,20 +4350,20 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>11/09/2019</t>
+          <t>03/11/2021</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>13/09/2019</t>
+          <t>17/12/2021</t>
         </is>
       </c>
       <c r="D146" t="n">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
-          <t>RECOMISSIONAMENTO REGULADORES</t>
+          <t>CAVITAÇÃO</t>
         </is>
       </c>
       <c r="F146" t="inlineStr"/>
@@ -4385,20 +4377,20 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>17/09/2019</t>
+          <t>17/06/2022</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>31/10/2019</t>
+          <t>19/06/2022</t>
         </is>
       </c>
       <c r="D147" t="n">
-        <v>45</v>
+        <v>3</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
-          <t>CAVITAÇÃO</t>
+          <t>RECOMISSIONAMENTO REGULADORES</t>
         </is>
       </c>
       <c r="F147" t="inlineStr"/>
@@ -4407,25 +4399,25 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>ROUHSN_13P8_UG49</t>
+          <t>ROUHSN_13P8_UG50</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>16/11/2019</t>
+          <t>02/09/2021</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>06/12/2019</t>
+          <t>21/09/2021</t>
         </is>
       </c>
       <c r="D148" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
-          <t>VEDAÇÃO DO EIXO</t>
+          <t>VEDAÇÃO DO EIXO (ILHA 01)</t>
         </is>
       </c>
       <c r="F148" t="inlineStr"/>
@@ -4439,20 +4431,20 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>18/07/2019</t>
+          <t>19/10/2021</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>06/08/2019</t>
+          <t>14/11/2021</t>
         </is>
       </c>
       <c r="D149" t="n">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
-          <t>VEDAÇÃO DO EIXO (ILHA 01)</t>
+          <t>MANUTENÇÃO CORRETIVA VEDAÇÃO DO EIXO</t>
         </is>
       </c>
       <c r="F149" t="inlineStr"/>
@@ -4466,12 +4458,12 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>15/08/2019</t>
+          <t>22/12/2021</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>28/08/2019</t>
+          <t>04/01/2022</t>
         </is>
       </c>
       <c r="D150" t="n">
@@ -4488,25 +4480,17 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>ROUHSN_13P8_UG50</t>
-        </is>
-      </c>
-      <c r="B151" t="inlineStr">
-        <is>
-          <t>08/09/2019</t>
-        </is>
-      </c>
-      <c r="C151" t="inlineStr">
-        <is>
-          <t>04/10/2019</t>
-        </is>
-      </c>
+          <t>ROUHSN_13P8_UG01</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr"/>
+      <c r="C151" t="inlineStr"/>
       <c r="D151" t="n">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
-          <t>MANUTENÇÃO CORRETIVA VEDAÇÃO DO EIXO</t>
+          <t>BIELISMO ROTOR KAPLAN</t>
         </is>
       </c>
       <c r="F151" t="inlineStr"/>
@@ -4515,15 +4499,17 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>ROUHSN_13P8_UG03</t>
+          <t>ROUHSN_13P8_UG01</t>
         </is>
       </c>
       <c r="B152" t="inlineStr"/>
       <c r="C152" t="inlineStr"/>
-      <c r="D152" t="inlineStr"/>
+      <c r="D152" t="n">
+        <v>29</v>
+      </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>MANUTENÇÃO CORRETIVA SISTEMA REG VEL</t>
+          <t>MANUTENÇÃO CORRETIVA VEDAÇÃO DO EIXO</t>
         </is>
       </c>
       <c r="F152" t="inlineStr"/>
@@ -4532,17 +4518,15 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>ROUHSN_13P8_UG09</t>
+          <t>ROUHSN_13P8_UG03</t>
         </is>
       </c>
       <c r="B153" t="inlineStr"/>
       <c r="C153" t="inlineStr"/>
-      <c r="D153" t="n">
-        <v>23</v>
-      </c>
+      <c r="D153" t="inlineStr"/>
       <c r="E153" t="inlineStr">
         <is>
-          <t>INSPEÇÃO NOS MANCIAS</t>
+          <t>MANUTENÇÃO CORRETIVA SISTEMA REG VEL</t>
         </is>
       </c>
       <c r="F153" t="inlineStr"/>
@@ -4591,11 +4575,11 @@
       <c r="B156" t="inlineStr"/>
       <c r="C156" t="inlineStr"/>
       <c r="D156" t="n">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
-          <t>MANUTENÇÃO CORRETIVA VEDAÇÃO DO EIXO</t>
+          <t>BIELISMO ROTOR KAPLAN</t>
         </is>
       </c>
       <c r="F156" t="inlineStr"/>
@@ -4610,15 +4594,91 @@
       <c r="B157" t="inlineStr"/>
       <c r="C157" t="inlineStr"/>
       <c r="D157" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E157" t="inlineStr">
         <is>
-          <t>PARADA DA ILHA - TRANSFORMADOR</t>
+          <t>ENSAIO DE RENDIMENTO</t>
         </is>
       </c>
       <c r="F157" t="inlineStr"/>
       <c r="G157" t="inlineStr"/>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>ROUHSN_13P8_UG29</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr"/>
+      <c r="C158" t="inlineStr"/>
+      <c r="D158" t="n">
+        <v>31</v>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>VEDAÇÃO DO EIXO</t>
+        </is>
+      </c>
+      <c r="F158" t="inlineStr"/>
+      <c r="G158" t="inlineStr"/>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>ROUHSN_13P8_UG29</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr"/>
+      <c r="C159" t="inlineStr"/>
+      <c r="D159" t="n">
+        <v>27</v>
+      </c>
+      <c r="E159" t="inlineStr">
+        <is>
+          <t>SUBSTITUIÇÃO DE TRUG</t>
+        </is>
+      </c>
+      <c r="F159" t="inlineStr"/>
+      <c r="G159" t="inlineStr"/>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>ROUHSN_13P8_UG42</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr"/>
+      <c r="C160" t="inlineStr"/>
+      <c r="D160" t="n">
+        <v>26</v>
+      </c>
+      <c r="E160" t="inlineStr">
+        <is>
+          <t>VEDAÇÃO DO EIXO (ILHA 02)</t>
+        </is>
+      </c>
+      <c r="F160" t="inlineStr"/>
+      <c r="G160" t="inlineStr"/>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>ROUHSN_13P8_UG42</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr"/>
+      <c r="C161" t="inlineStr"/>
+      <c r="D161" t="n">
+        <v>57</v>
+      </c>
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>MANUTENÇÃO CORRETIVA TUBULAÇÃO KAPLAN</t>
+        </is>
+      </c>
+      <c r="F161" t="inlineStr"/>
+      <c r="G161" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>